<commit_message>
UPdate Orders.xlsx with latest data
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="970">
   <si>
     <t>Order Number</t>
   </si>
@@ -2498,6 +2498,653 @@
   </si>
   <si>
     <t>03107301569</t>
+  </si>
+  <si>
+    <t>3016</t>
+  </si>
+  <si>
+    <t>Distt karak not present in your list. Please add...
+My add.sami khan
+Danyal medical store near UBL Karak
+Kpk.03005998988</t>
+  </si>
+  <si>
+    <t>Sami khan</t>
+  </si>
+  <si>
+    <t>Danyal medical store near ubl karak</t>
+  </si>
+  <si>
+    <t>Peshawar District</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>drsamiullah36@gmail.com</t>
+  </si>
+  <si>
+    <t>03005998988</t>
+  </si>
+  <si>
+    <t>Sahel F-1 ساحل
+T0-1057 ٹماٹر
+Smilla پھول گوبھی
+Super Green كريلا
+Slowbolt دھنیا</t>
+  </si>
+  <si>
+    <t>5000
+3588
+2104
+2852
+575</t>
+  </si>
+  <si>
+    <t>3017</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>Arafat computers</t>
+  </si>
+  <si>
+    <t>Arafat Computers Shop No 6# Faiz Muhammad Road Near Liaquat Bazzar Quetta Balochistan, Arafat Computers Shop No 6# Faiz Muhammad Road</t>
+  </si>
+  <si>
+    <t>87300</t>
+  </si>
+  <si>
+    <t>arafatcomputers@yahoo.com</t>
+  </si>
+  <si>
+    <t>+923003880119</t>
+  </si>
+  <si>
+    <t>3018</t>
+  </si>
+  <si>
+    <t>Hamza</t>
+  </si>
+  <si>
+    <t>Just for testing purpose</t>
+  </si>
+  <si>
+    <t>Street 123</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>03460000000</t>
+  </si>
+  <si>
+    <t>3019</t>
+  </si>
+  <si>
+    <t>Rajana road toba, Shaukat khanum laboratory collection center</t>
+  </si>
+  <si>
+    <t>3600</t>
+  </si>
+  <si>
+    <t>asifbsp@gmail.com</t>
+  </si>
+  <si>
+    <t>03112693131</t>
+  </si>
+  <si>
+    <t>3021</t>
+  </si>
+  <si>
+    <t>Waseem</t>
+  </si>
+  <si>
+    <t>Mehar</t>
+  </si>
+  <si>
+    <t>Mehar House Near Mirch Mndi Asif nagr Kunri, Mirch mndi</t>
+  </si>
+  <si>
+    <t>69160</t>
+  </si>
+  <si>
+    <t>mehartractor@gmail.com</t>
+  </si>
+  <si>
+    <t>03003300944</t>
+  </si>
+  <si>
+    <t>Hot Pepper رائل ریڈ
+Slowbolt دھنیا</t>
+  </si>
+  <si>
+    <t>4876
+575</t>
+  </si>
+  <si>
+    <t>3022</t>
+  </si>
+  <si>
+    <t>Musadiq</t>
+  </si>
+  <si>
+    <t>Azim</t>
+  </si>
+  <si>
+    <t>Farming</t>
+  </si>
+  <si>
+    <t>Tcs office RCD road khuzdar</t>
+  </si>
+  <si>
+    <t>Khuzdar District</t>
+  </si>
+  <si>
+    <t>musadiqazim123@gmail.com</t>
+  </si>
+  <si>
+    <t>03432852363</t>
+  </si>
+  <si>
+    <t>3023</t>
+  </si>
+  <si>
+    <t>Muhammadshahzad</t>
+  </si>
+  <si>
+    <t>Shahzad</t>
+  </si>
+  <si>
+    <t>Mouza FazilShah Post office sardar pur Tehsil Kabirwala District Khanewal</t>
+  </si>
+  <si>
+    <t>mshahzad5566990@gmail.com</t>
+  </si>
+  <si>
+    <t>03417299200</t>
+  </si>
+  <si>
+    <t>Melon خربوزہ</t>
+  </si>
+  <si>
+    <t>3024</t>
+  </si>
+  <si>
+    <t>Arshad</t>
+  </si>
+  <si>
+    <t>Mehmood</t>
+  </si>
+  <si>
+    <t>Pak cng filling station, Basal Road Attock</t>
+  </si>
+  <si>
+    <t>arshadmahmoodkhan.57@gmail.com</t>
+  </si>
+  <si>
+    <t>03005262723</t>
+  </si>
+  <si>
+    <t>TAI-1156 ٹماٹر
+Bonny پھول گوبھی</t>
+  </si>
+  <si>
+    <t>5060
+4876</t>
+  </si>
+  <si>
+    <t>3025</t>
+  </si>
+  <si>
+    <t>Zuhak</t>
+  </si>
+  <si>
+    <t>House no c286 Ward no 03 near Madina masjid kot gulam Muhammad</t>
+  </si>
+  <si>
+    <t>aijazkk66@gmail.com</t>
+  </si>
+  <si>
+    <t>03172837476</t>
+  </si>
+  <si>
+    <t>3026</t>
+  </si>
+  <si>
+    <t>Kb tk deliver ho ga</t>
+  </si>
+  <si>
+    <t>Rao Abdul</t>
+  </si>
+  <si>
+    <t>Waheed khan</t>
+  </si>
+  <si>
+    <t>Kissan zari services</t>
+  </si>
+  <si>
+    <t>Chak no 72/15L khanewal, Nzd Ada choke Jamal</t>
+  </si>
+  <si>
+    <t>Hot Pepper رائل ریڈ</t>
+  </si>
+  <si>
+    <t>3027</t>
+  </si>
+  <si>
+    <t>61/2, Khayaban E Ittehad Phase 6 Dha</t>
+  </si>
+  <si>
+    <t>75500</t>
+  </si>
+  <si>
+    <t>ahmedhn5@gmail.com</t>
+  </si>
+  <si>
+    <t>03332149932</t>
+  </si>
+  <si>
+    <t>3028</t>
+  </si>
+  <si>
+    <t>Rana</t>
+  </si>
+  <si>
+    <t>wali ullah Wali Ullah</t>
+  </si>
+  <si>
+    <t>Lucky Filling Station Feroz Wattoan District &amp; Tehsel Shekhupura</t>
+  </si>
+  <si>
+    <t>walliullahjoiya@icloud.com</t>
+  </si>
+  <si>
+    <t>03024440223</t>
+  </si>
+  <si>
+    <t>3029</t>
+  </si>
+  <si>
+    <t>Amin</t>
+  </si>
+  <si>
+    <t>Royal Roller Flour Mills Pvt Ltd, Baradari Road, Chowk Begum Kot, Shahdara, Lahore</t>
+  </si>
+  <si>
+    <t>54000</t>
+  </si>
+  <si>
+    <t>matifamin@hotmail.com</t>
+  </si>
+  <si>
+    <t>03334888808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>1
+2
+3
+4
+5
+6
+7
+8
+9
+10</t>
+  </si>
+  <si>
+    <t>TAI-14-6242 ٹماٹر
+Smilla پھول گوبھی
+Roshni مرچ
+Orobelle شملہ مرچ
+Maxwell کھیرا
+Champion كريلا
+Purple Top White Globe شلجم
+Round Red مولی
+Sahel F-1 ساحل
+Slowbolt دھنیا</t>
+  </si>
+  <si>
+    <t>1
+1
+1
+1
+1
+1
+1
+1
+1
+1</t>
+  </si>
+  <si>
+    <t>3864
+2104
+2928
+3496
+6256
+2852
+1300
+1700
+5000
+575</t>
+  </si>
+  <si>
+    <t>3030</t>
+  </si>
+  <si>
+    <t>Syed</t>
+  </si>
+  <si>
+    <t>Ahmed Waleed</t>
+  </si>
+  <si>
+    <t>House number 65 falcon complex 68 the mall road Peshawar Cantt</t>
+  </si>
+  <si>
+    <t>waleed_syed@live.com</t>
+  </si>
+  <si>
+    <t>03332218080</t>
+  </si>
+  <si>
+    <t>3031</t>
+  </si>
+  <si>
+    <t>3032</t>
+  </si>
+  <si>
+    <t>3033</t>
+  </si>
+  <si>
+    <t>Aleem</t>
+  </si>
+  <si>
+    <t>Hameed Khan</t>
+  </si>
+  <si>
+    <t>Village Gul Muhammad brohi</t>
+  </si>
+  <si>
+    <t>hameed356.f@gmail.com</t>
+  </si>
+  <si>
+    <t>03093842458</t>
+  </si>
+  <si>
+    <t>3037</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Sas156</t>
+  </si>
+  <si>
+    <t>Churjamli, House 1</t>
+  </si>
+  <si>
+    <t>73070</t>
+  </si>
+  <si>
+    <t>ahmadking1561723@gmail.com</t>
+  </si>
+  <si>
+    <t>03098495340</t>
+  </si>
+  <si>
+    <t>3038</t>
+  </si>
+  <si>
+    <t>Zaid</t>
+  </si>
+  <si>
+    <t>Muhammad Zaid</t>
+  </si>
+  <si>
+    <t>Bahawalnagar</t>
+  </si>
+  <si>
+    <t>62300</t>
+  </si>
+  <si>
+    <t>abdulrazzaq8690201@gmail.com</t>
+  </si>
+  <si>
+    <t>03055838888</t>
+  </si>
+  <si>
+    <t>3039</t>
+  </si>
+  <si>
+    <t>Noman</t>
+  </si>
+  <si>
+    <t>Chak# 32 JB</t>
+  </si>
+  <si>
+    <t>miannoman323232@gmail.com</t>
+  </si>
+  <si>
+    <t>+923499567031</t>
+  </si>
+  <si>
+    <t>3041</t>
+  </si>
+  <si>
+    <t>Jeesing</t>
+  </si>
+  <si>
+    <t>03423237255, 112233</t>
+  </si>
+  <si>
+    <t>112233</t>
+  </si>
+  <si>
+    <t>jeesingkholi@gmail.com</t>
+  </si>
+  <si>
+    <t>03423237255</t>
+  </si>
+  <si>
+    <t>3042</t>
+  </si>
+  <si>
+    <t>Ihsan</t>
+  </si>
+  <si>
+    <t>Anas stores</t>
+  </si>
+  <si>
+    <t>Shah super store Tindodag swat, Village council office</t>
+  </si>
+  <si>
+    <t>4444</t>
+  </si>
+  <si>
+    <t>ihsanali35@yahoo.com</t>
+  </si>
+  <si>
+    <t>03414047881</t>
+  </si>
+  <si>
+    <t>3043</t>
+  </si>
+  <si>
+    <t>Abdullah</t>
+  </si>
+  <si>
+    <t>MuhammadAbdullah</t>
+  </si>
+  <si>
+    <t>MuhammadAbdullah 03225914546</t>
+  </si>
+  <si>
+    <t>078632abdullah@gmail.com</t>
+  </si>
+  <si>
+    <t>+613225914546</t>
+  </si>
+  <si>
+    <t>3046</t>
+  </si>
+  <si>
+    <t>Hot Pepper رائل ریڈ
+Orobelle شملہ مرچ
+Slowbolt دھنیا</t>
+  </si>
+  <si>
+    <t>4876
+3496
+575</t>
+  </si>
+  <si>
+    <t>3047</t>
+  </si>
+  <si>
+    <t>Jinsar Ali</t>
+  </si>
+  <si>
+    <t>Khoso</t>
+  </si>
+  <si>
+    <t>Jinsar Ali Khoso</t>
+  </si>
+  <si>
+    <t>03147406312</t>
+  </si>
+  <si>
+    <t>JK</t>
+  </si>
+  <si>
+    <t>03127406312</t>
+  </si>
+  <si>
+    <t>jinsaralikhoso89@gmail.com</t>
+  </si>
+  <si>
+    <t>3048</t>
+  </si>
+  <si>
+    <t>Ward no 10 mohalla Sadat</t>
+  </si>
+  <si>
+    <t>3049</t>
+  </si>
+  <si>
+    <t>Mohsin</t>
+  </si>
+  <si>
+    <t>Bookshop</t>
+  </si>
+  <si>
+    <t>Mohsin bookshop Samundri</t>
+  </si>
+  <si>
+    <t>mohsanrana4467@gmail.com</t>
+  </si>
+  <si>
+    <t>03225328261</t>
+  </si>
+  <si>
+    <t>3053</t>
+  </si>
+  <si>
+    <t>Allah</t>
+  </si>
+  <si>
+    <t>Bux</t>
+  </si>
+  <si>
+    <t>Allah Bux</t>
+  </si>
+  <si>
+    <t>Basti Arab</t>
+  </si>
+  <si>
+    <t>03058407985</t>
+  </si>
+  <si>
+    <t>3054</t>
+  </si>
+  <si>
+    <t>Qamar</t>
+  </si>
+  <si>
+    <t>Jazz Franchise Near ubl bank pindi Road talagang</t>
+  </si>
+  <si>
+    <t>qamarabbas308@gmail.com</t>
+  </si>
+  <si>
+    <t>03028429987</t>
+  </si>
+  <si>
+    <t>Slowbolt دھنیا
+CFH1522 پھول گوبھی
+BC-90 بند گوبھی</t>
+  </si>
+  <si>
+    <t>575
+2070
+3294</t>
+  </si>
+  <si>
+    <t>3056</t>
+  </si>
+  <si>
+    <t>Mohalla Langer khail Kokarai Swat</t>
+  </si>
+  <si>
+    <t>19130</t>
+  </si>
+  <si>
+    <t>naveedhateler143@gmail.com</t>
+  </si>
+  <si>
+    <t>03463373336</t>
+  </si>
+  <si>
+    <t>3059</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Xyz</t>
+  </si>
+  <si>
+    <t>Abc, Aaaa</t>
+  </si>
+  <si>
+    <t>12322</t>
+  </si>
+  <si>
+    <t>+923354912148</t>
+  </si>
+  <si>
+    <t>Hot Pepper رائل ریڈ
+TAI-14-6242 ٹماٹر</t>
+  </si>
+  <si>
+    <t>4876
+3864</t>
+  </si>
+  <si>
+    <t>3060</t>
+  </si>
+  <si>
+    <t>5400</t>
+  </si>
+  <si>
+    <t>3061</t>
+  </si>
+  <si>
+    <t>Jazz franchise near ubl bank pindi Road talagang, Jazz franchise near ubl bank pindi Road talagang</t>
   </si>
 </sst>
 </file>
@@ -2865,7 +3512,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AL115"/>
+  <dimension ref="A1:AL148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="1" activePane="bottomLeft" state="frozen" topLeftCell="A2"/>
@@ -2879,7 +3526,7 @@
     <col min="3" max="3" width="19.995" bestFit="true" customWidth="true" style="5"/>
     <col min="4" max="4" width="209.949" bestFit="true" customWidth="true" style="3"/>
     <col min="5" max="5" width="25.851" bestFit="true" customWidth="true" style="3"/>
-    <col min="6" max="6" width="23.423" bestFit="true" customWidth="true" style="3"/>
+    <col min="6" max="6" width="25.851" bestFit="true" customWidth="true" style="3"/>
     <col min="7" max="7" width="43.561" bestFit="true" customWidth="true" style="3"/>
     <col min="8" max="8" width="172.101" bestFit="true" customWidth="true" style="3"/>
     <col min="9" max="9" width="29.421" bestFit="true" customWidth="true" style="3"/>
@@ -2889,7 +3536,7 @@
     <col min="13" max="13" width="38.848" bestFit="true" customWidth="true" style="3"/>
     <col min="14" max="14" width="18.71" bestFit="true" customWidth="true" style="3"/>
     <col min="15" max="15" width="25.851" bestFit="true" customWidth="true" style="3"/>
-    <col min="16" max="16" width="24.708" bestFit="true" customWidth="true" style="3"/>
+    <col min="16" max="16" width="25.851" bestFit="true" customWidth="true" style="3"/>
     <col min="17" max="17" width="172.101" bestFit="true" customWidth="true" style="3"/>
     <col min="18" max="18" width="29.421" bestFit="true" customWidth="true" style="3"/>
     <col min="19" max="19" width="25.851" bestFit="true" customWidth="true" style="3"/>
@@ -11905,7 +12552,7 @@
         <v>636</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>51</v>
+        <v>311</v>
       </c>
       <c r="C90" s="5">
         <v>45846.570902778</v>
@@ -13343,7 +13990,7 @@
         <v>716</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C104" s="5">
         <v>45852.165729167</v>
@@ -14275,7 +14922,7 @@
         <v>762</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C113" s="5">
         <v>45854.537349537</v>
@@ -14377,7 +15024,7 @@
         <v>770</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C114" s="5">
         <v>45854.547037037</v>
@@ -14567,6 +15214,3348 @@
         <v>575.0</v>
       </c>
       <c r="AJ115" s="3"/>
+    </row>
+    <row r="116" spans="1:38">
+      <c r="A116" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C116" s="5">
+        <v>45857.557395833</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M116" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="N116" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="O116" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="P116" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q116" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T116" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W116">
+        <v>0</v>
+      </c>
+      <c r="X116">
+        <v>0.0</v>
+      </c>
+      <c r="Y116">
+        <v>14119.0</v>
+      </c>
+      <c r="Z116" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA116">
+        <v>300</v>
+      </c>
+      <c r="AB116">
+        <v>0</v>
+      </c>
+      <c r="AC116">
+        <v>14419</v>
+      </c>
+      <c r="AD116">
+        <v>0.0</v>
+      </c>
+      <c r="AE116" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="AF116" t="s">
+        <v>614</v>
+      </c>
+      <c r="AG116" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="AH116" t="s">
+        <v>616</v>
+      </c>
+      <c r="AI116" t="s">
+        <v>784</v>
+      </c>
+      <c r="AJ116" s="3"/>
+    </row>
+    <row r="117" spans="1:38">
+      <c r="A117" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C117" s="5">
+        <v>45857.774918981</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="L117" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M117" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="N117" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="O117" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="P117" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q117" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="R117" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="S117" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="T117" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="U117" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V117" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W117">
+        <v>0</v>
+      </c>
+      <c r="X117">
+        <v>0.0</v>
+      </c>
+      <c r="Y117">
+        <v>18768.0</v>
+      </c>
+      <c r="Z117" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA117">
+        <v>300</v>
+      </c>
+      <c r="AB117">
+        <v>0</v>
+      </c>
+      <c r="AC117">
+        <v>19068</v>
+      </c>
+      <c r="AD117">
+        <v>0.0</v>
+      </c>
+      <c r="AE117" s="3"/>
+      <c r="AF117">
+        <v>1</v>
+      </c>
+      <c r="AG117" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="AH117">
+        <v>3</v>
+      </c>
+      <c r="AI117">
+        <v>6256.0</v>
+      </c>
+      <c r="AJ117" s="3"/>
+    </row>
+    <row r="118" spans="1:38">
+      <c r="A118" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C118" s="5">
+        <v>45858.172997685</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M118" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="N118" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="O118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P118" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="Q118" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T118" s="3"/>
+      <c r="U118" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W118">
+        <v>0</v>
+      </c>
+      <c r="X118">
+        <v>0.0</v>
+      </c>
+      <c r="Y118">
+        <v>575.0</v>
+      </c>
+      <c r="Z118" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA118">
+        <v>300</v>
+      </c>
+      <c r="AB118">
+        <v>0</v>
+      </c>
+      <c r="AC118">
+        <v>875</v>
+      </c>
+      <c r="AD118">
+        <v>0.0</v>
+      </c>
+      <c r="AE118" s="3"/>
+      <c r="AF118">
+        <v>1</v>
+      </c>
+      <c r="AG118" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH118">
+        <v>1</v>
+      </c>
+      <c r="AI118">
+        <v>575.0</v>
+      </c>
+      <c r="AJ118" s="3"/>
+    </row>
+    <row r="119" spans="1:38">
+      <c r="A119" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C119" s="5">
+        <v>45858.420775463</v>
+      </c>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K119" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="L119" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M119" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="N119" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="O119" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P119" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="Q119" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="R119" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="S119" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T119" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="U119" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V119" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W119">
+        <v>0</v>
+      </c>
+      <c r="X119">
+        <v>0.0</v>
+      </c>
+      <c r="Y119">
+        <v>2852.0</v>
+      </c>
+      <c r="Z119" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA119">
+        <v>300</v>
+      </c>
+      <c r="AB119">
+        <v>0</v>
+      </c>
+      <c r="AC119">
+        <v>3152</v>
+      </c>
+      <c r="AD119">
+        <v>0.0</v>
+      </c>
+      <c r="AE119" s="3"/>
+      <c r="AF119">
+        <v>1</v>
+      </c>
+      <c r="AG119" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="AH119">
+        <v>1</v>
+      </c>
+      <c r="AI119">
+        <v>2852.0</v>
+      </c>
+      <c r="AJ119" s="3"/>
+    </row>
+    <row r="120" spans="1:38">
+      <c r="A120" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C120" s="5">
+        <v>45859.238171296</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K120" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="L120" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M120" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="N120" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="O120" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="P120" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="Q120" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T120" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W120">
+        <v>0</v>
+      </c>
+      <c r="X120">
+        <v>0.0</v>
+      </c>
+      <c r="Y120">
+        <v>5451.0</v>
+      </c>
+      <c r="Z120" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA120">
+        <v>300</v>
+      </c>
+      <c r="AB120">
+        <v>0</v>
+      </c>
+      <c r="AC120">
+        <v>5751</v>
+      </c>
+      <c r="AD120">
+        <v>0.0</v>
+      </c>
+      <c r="AE120" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF120" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG120" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="AH120" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI120" t="s">
+        <v>811</v>
+      </c>
+      <c r="AJ120" s="3"/>
+    </row>
+    <row r="121" spans="1:38">
+      <c r="A121" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C121" s="5">
+        <v>45859.258125</v>
+      </c>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M121" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="N121" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="O121" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="P121" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="Q121" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="R121" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="S121" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="T121" s="3"/>
+      <c r="U121" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V121" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W121">
+        <v>0</v>
+      </c>
+      <c r="X121">
+        <v>0.0</v>
+      </c>
+      <c r="Y121">
+        <v>5000.0</v>
+      </c>
+      <c r="Z121" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA121">
+        <v>300</v>
+      </c>
+      <c r="AB121">
+        <v>0</v>
+      </c>
+      <c r="AC121">
+        <v>5300</v>
+      </c>
+      <c r="AD121">
+        <v>0.0</v>
+      </c>
+      <c r="AE121" s="3"/>
+      <c r="AF121">
+        <v>1</v>
+      </c>
+      <c r="AG121" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH121">
+        <v>1</v>
+      </c>
+      <c r="AI121">
+        <v>5000.0</v>
+      </c>
+      <c r="AJ121" s="3"/>
+    </row>
+    <row r="122" spans="1:38">
+      <c r="A122" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C122" s="5">
+        <v>45859.406331019</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M122" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="N122" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="O122" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="P122" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="Q122" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T122" s="3"/>
+      <c r="U122" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W122">
+        <v>0</v>
+      </c>
+      <c r="X122">
+        <v>0.0</v>
+      </c>
+      <c r="Y122">
+        <v>5490.0</v>
+      </c>
+      <c r="Z122" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA122">
+        <v>300</v>
+      </c>
+      <c r="AB122">
+        <v>0</v>
+      </c>
+      <c r="AC122">
+        <v>5790</v>
+      </c>
+      <c r="AD122">
+        <v>0.0</v>
+      </c>
+      <c r="AE122" s="3"/>
+      <c r="AF122">
+        <v>1</v>
+      </c>
+      <c r="AG122" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="AH122">
+        <v>1</v>
+      </c>
+      <c r="AI122">
+        <v>5490.0</v>
+      </c>
+      <c r="AJ122" s="3"/>
+    </row>
+    <row r="123" spans="1:38">
+      <c r="A123" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C123" s="5">
+        <v>45859.57755787</v>
+      </c>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K123" s="3"/>
+      <c r="L123" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M123" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="O123" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="P123" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="Q123" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="R123" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="S123" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T123" s="3"/>
+      <c r="U123" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V123" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W123">
+        <v>0</v>
+      </c>
+      <c r="X123">
+        <v>0.0</v>
+      </c>
+      <c r="Y123">
+        <v>9936.0</v>
+      </c>
+      <c r="Z123" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA123">
+        <v>300</v>
+      </c>
+      <c r="AB123">
+        <v>0</v>
+      </c>
+      <c r="AC123">
+        <v>10236</v>
+      </c>
+      <c r="AD123">
+        <v>0.0</v>
+      </c>
+      <c r="AE123" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF123" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG123" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="AH123" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI123" t="s">
+        <v>834</v>
+      </c>
+      <c r="AJ123" s="3"/>
+    </row>
+    <row r="124" spans="1:38">
+      <c r="A124" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C124" s="5">
+        <v>45859.701180556</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M124" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="N124" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="O124" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P124" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="Q124" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T124" s="3"/>
+      <c r="U124" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W124">
+        <v>0</v>
+      </c>
+      <c r="X124">
+        <v>0.0</v>
+      </c>
+      <c r="Y124">
+        <v>1725.0</v>
+      </c>
+      <c r="Z124" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA124">
+        <v>300</v>
+      </c>
+      <c r="AB124">
+        <v>0</v>
+      </c>
+      <c r="AC124">
+        <v>2025</v>
+      </c>
+      <c r="AD124">
+        <v>0.0</v>
+      </c>
+      <c r="AE124" s="3"/>
+      <c r="AF124">
+        <v>1</v>
+      </c>
+      <c r="AG124" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH124">
+        <v>3</v>
+      </c>
+      <c r="AI124">
+        <v>575.0</v>
+      </c>
+      <c r="AJ124" s="3"/>
+    </row>
+    <row r="125" spans="1:38">
+      <c r="A125" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C125" s="5">
+        <v>45860.241261574</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K125" s="3"/>
+      <c r="L125" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M125" s="3"/>
+      <c r="N125" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="O125" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="P125" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="Q125" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="R125" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="S125" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T125" s="3"/>
+      <c r="U125" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V125" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W125">
+        <v>0</v>
+      </c>
+      <c r="X125">
+        <v>0.0</v>
+      </c>
+      <c r="Y125">
+        <v>4876.0</v>
+      </c>
+      <c r="Z125" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA125">
+        <v>300</v>
+      </c>
+      <c r="AB125">
+        <v>0</v>
+      </c>
+      <c r="AC125">
+        <v>5176</v>
+      </c>
+      <c r="AD125">
+        <v>0.0</v>
+      </c>
+      <c r="AE125" s="3"/>
+      <c r="AF125">
+        <v>1</v>
+      </c>
+      <c r="AG125" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="AH125">
+        <v>1</v>
+      </c>
+      <c r="AI125">
+        <v>4876.0</v>
+      </c>
+      <c r="AJ125" s="3"/>
+    </row>
+    <row r="126" spans="1:38">
+      <c r="A126" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C126" s="5">
+        <v>45860.39162037</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="L126" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M126" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="N126" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="O126" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="P126" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q126" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T126" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W126">
+        <v>0</v>
+      </c>
+      <c r="X126">
+        <v>0.0</v>
+      </c>
+      <c r="Y126">
+        <v>3864.0</v>
+      </c>
+      <c r="Z126" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA126">
+        <v>300</v>
+      </c>
+      <c r="AB126">
+        <v>0</v>
+      </c>
+      <c r="AC126">
+        <v>4164</v>
+      </c>
+      <c r="AD126">
+        <v>0.0</v>
+      </c>
+      <c r="AE126" s="3"/>
+      <c r="AF126">
+        <v>1</v>
+      </c>
+      <c r="AG126" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH126">
+        <v>1</v>
+      </c>
+      <c r="AI126">
+        <v>3864.0</v>
+      </c>
+      <c r="AJ126" s="3"/>
+    </row>
+    <row r="127" spans="1:38">
+      <c r="A127" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C127" s="5">
+        <v>45861.469918981</v>
+      </c>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="J127" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K127" s="3"/>
+      <c r="L127" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M127" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="N127" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="O127" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="P127" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="Q127" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="R127" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="S127" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T127" s="3"/>
+      <c r="U127" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V127" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W127">
+        <v>0</v>
+      </c>
+      <c r="X127">
+        <v>0.0</v>
+      </c>
+      <c r="Y127">
+        <v>20700.0</v>
+      </c>
+      <c r="Z127" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA127">
+        <v>300</v>
+      </c>
+      <c r="AB127">
+        <v>0</v>
+      </c>
+      <c r="AC127">
+        <v>21000</v>
+      </c>
+      <c r="AD127">
+        <v>0.0</v>
+      </c>
+      <c r="AE127" s="3"/>
+      <c r="AF127">
+        <v>1</v>
+      </c>
+      <c r="AG127" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH127">
+        <v>10</v>
+      </c>
+      <c r="AI127">
+        <v>2070.0</v>
+      </c>
+      <c r="AJ127" s="3"/>
+    </row>
+    <row r="128" spans="1:38">
+      <c r="A128" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C128" s="5">
+        <v>45862.204340278</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="G128" s="3"/>
+      <c r="H128" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="L128" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M128" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="N128" s="3" t="s">
+        <v>863</v>
+      </c>
+      <c r="O128" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="P128" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="Q128" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T128" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W128">
+        <v>0</v>
+      </c>
+      <c r="X128">
+        <v>0.0</v>
+      </c>
+      <c r="Y128">
+        <v>30075.0</v>
+      </c>
+      <c r="Z128" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA128">
+        <v>300</v>
+      </c>
+      <c r="AB128">
+        <v>0</v>
+      </c>
+      <c r="AC128">
+        <v>30375</v>
+      </c>
+      <c r="AD128">
+        <v>0.0</v>
+      </c>
+      <c r="AE128" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="AF128" t="s">
+        <v>865</v>
+      </c>
+      <c r="AG128" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="AH128" t="s">
+        <v>867</v>
+      </c>
+      <c r="AI128" t="s">
+        <v>868</v>
+      </c>
+      <c r="AJ128" s="3"/>
+    </row>
+    <row r="129" spans="1:38">
+      <c r="A129" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C129" s="5">
+        <v>45862.258819444</v>
+      </c>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K129" s="3"/>
+      <c r="L129" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M129" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="N129" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="O129" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="P129" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="Q129" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="R129" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="S129" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T129" s="3"/>
+      <c r="U129" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V129" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W129">
+        <v>0</v>
+      </c>
+      <c r="X129">
+        <v>0.0</v>
+      </c>
+      <c r="Y129">
+        <v>3864.0</v>
+      </c>
+      <c r="Z129" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA129">
+        <v>300</v>
+      </c>
+      <c r="AB129">
+        <v>0</v>
+      </c>
+      <c r="AC129">
+        <v>4164</v>
+      </c>
+      <c r="AD129">
+        <v>0.0</v>
+      </c>
+      <c r="AE129" s="3"/>
+      <c r="AF129">
+        <v>1</v>
+      </c>
+      <c r="AG129" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH129">
+        <v>1</v>
+      </c>
+      <c r="AI129">
+        <v>3864.0</v>
+      </c>
+      <c r="AJ129" s="3"/>
+    </row>
+    <row r="130" spans="1:38">
+      <c r="A130" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C130" s="5">
+        <v>45862.460023148</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="G130" s="3"/>
+      <c r="H130" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M130" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="N130" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="O130" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="P130" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="Q130" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T130" s="3"/>
+      <c r="U130" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W130">
+        <v>0</v>
+      </c>
+      <c r="X130">
+        <v>0.0</v>
+      </c>
+      <c r="Y130">
+        <v>3864.0</v>
+      </c>
+      <c r="Z130" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA130">
+        <v>300</v>
+      </c>
+      <c r="AB130">
+        <v>0</v>
+      </c>
+      <c r="AC130">
+        <v>4164</v>
+      </c>
+      <c r="AD130">
+        <v>0.0</v>
+      </c>
+      <c r="AE130" s="3"/>
+      <c r="AF130">
+        <v>1</v>
+      </c>
+      <c r="AG130" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH130">
+        <v>1</v>
+      </c>
+      <c r="AI130">
+        <v>3864.0</v>
+      </c>
+      <c r="AJ130" s="3"/>
+    </row>
+    <row r="131" spans="1:38">
+      <c r="A131" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C131" s="5">
+        <v>45862.461481481</v>
+      </c>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K131" s="3"/>
+      <c r="L131" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M131" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="N131" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="O131" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="P131" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="Q131" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="R131" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="S131" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T131" s="3"/>
+      <c r="U131" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V131" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W131">
+        <v>0</v>
+      </c>
+      <c r="X131">
+        <v>0.0</v>
+      </c>
+      <c r="Y131">
+        <v>3864.0</v>
+      </c>
+      <c r="Z131" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA131">
+        <v>300</v>
+      </c>
+      <c r="AB131">
+        <v>0</v>
+      </c>
+      <c r="AC131">
+        <v>4164</v>
+      </c>
+      <c r="AD131">
+        <v>0.0</v>
+      </c>
+      <c r="AE131" s="3"/>
+      <c r="AF131">
+        <v>1</v>
+      </c>
+      <c r="AG131" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH131">
+        <v>1</v>
+      </c>
+      <c r="AI131">
+        <v>3864.0</v>
+      </c>
+      <c r="AJ131" s="3"/>
+    </row>
+    <row r="132" spans="1:38">
+      <c r="A132" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C132" s="5">
+        <v>45863.04505787</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M132" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="N132" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="O132" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="P132" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="Q132" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T132" s="3"/>
+      <c r="U132" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W132">
+        <v>0</v>
+      </c>
+      <c r="X132">
+        <v>0.0</v>
+      </c>
+      <c r="Y132">
+        <v>575.0</v>
+      </c>
+      <c r="Z132" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA132">
+        <v>300</v>
+      </c>
+      <c r="AB132">
+        <v>0</v>
+      </c>
+      <c r="AC132">
+        <v>875</v>
+      </c>
+      <c r="AD132">
+        <v>0.0</v>
+      </c>
+      <c r="AE132" s="3"/>
+      <c r="AF132">
+        <v>1</v>
+      </c>
+      <c r="AG132" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH132">
+        <v>1</v>
+      </c>
+      <c r="AI132">
+        <v>575.0</v>
+      </c>
+      <c r="AJ132" s="3"/>
+    </row>
+    <row r="133" spans="1:38">
+      <c r="A133" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C133" s="5">
+        <v>45865.194918981</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="L133" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M133" s="3" t="s">
+        <v>888</v>
+      </c>
+      <c r="N133" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="O133" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="P133" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q133" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="R133" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S133" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T133" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="U133" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V133" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W133">
+        <v>0</v>
+      </c>
+      <c r="X133">
+        <v>0.0</v>
+      </c>
+      <c r="Y133">
+        <v>89700.0</v>
+      </c>
+      <c r="Z133" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA133">
+        <v>300</v>
+      </c>
+      <c r="AB133">
+        <v>0</v>
+      </c>
+      <c r="AC133">
+        <v>90000</v>
+      </c>
+      <c r="AD133">
+        <v>0.0</v>
+      </c>
+      <c r="AE133" s="3"/>
+      <c r="AF133">
+        <v>1</v>
+      </c>
+      <c r="AG133" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH133">
+        <v>25</v>
+      </c>
+      <c r="AI133">
+        <v>3588.0</v>
+      </c>
+      <c r="AJ133" s="3"/>
+    </row>
+    <row r="134" spans="1:38">
+      <c r="A134" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C134" s="5">
+        <v>45865.478402778</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M134" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="N134" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="O134" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="P134" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q134" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T134" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W134">
+        <v>0</v>
+      </c>
+      <c r="X134">
+        <v>0.0</v>
+      </c>
+      <c r="Y134">
+        <v>575.0</v>
+      </c>
+      <c r="Z134" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA134">
+        <v>300</v>
+      </c>
+      <c r="AB134">
+        <v>0</v>
+      </c>
+      <c r="AC134">
+        <v>875</v>
+      </c>
+      <c r="AD134">
+        <v>0.0</v>
+      </c>
+      <c r="AE134" s="3"/>
+      <c r="AF134">
+        <v>1</v>
+      </c>
+      <c r="AG134" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH134">
+        <v>1</v>
+      </c>
+      <c r="AI134">
+        <v>575.0</v>
+      </c>
+      <c r="AJ134" s="3"/>
+    </row>
+    <row r="135" spans="1:38">
+      <c r="A135" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" s="5">
+        <v>45865.653125</v>
+      </c>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="J135" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M135" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="N135" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="O135" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="P135" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q135" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="R135" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="S135" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T135" s="3"/>
+      <c r="U135" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V135" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W135">
+        <v>0</v>
+      </c>
+      <c r="X135">
+        <v>0.0</v>
+      </c>
+      <c r="Y135">
+        <v>2070.0</v>
+      </c>
+      <c r="Z135" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA135">
+        <v>300</v>
+      </c>
+      <c r="AB135">
+        <v>0</v>
+      </c>
+      <c r="AC135">
+        <v>2370</v>
+      </c>
+      <c r="AD135">
+        <v>0.0</v>
+      </c>
+      <c r="AE135" s="3"/>
+      <c r="AF135">
+        <v>1</v>
+      </c>
+      <c r="AG135" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH135">
+        <v>1</v>
+      </c>
+      <c r="AI135">
+        <v>2070.0</v>
+      </c>
+      <c r="AJ135" s="3"/>
+    </row>
+    <row r="136" spans="1:38">
+      <c r="A136" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C136" s="5">
+        <v>45866.131863426</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M136" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="N136" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="O136" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="P136" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="Q136" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="R136" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="S136" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="T136" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="U136" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V136" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W136">
+        <v>0</v>
+      </c>
+      <c r="X136">
+        <v>0.0</v>
+      </c>
+      <c r="Y136">
+        <v>7728.0</v>
+      </c>
+      <c r="Z136" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA136">
+        <v>300</v>
+      </c>
+      <c r="AB136">
+        <v>0</v>
+      </c>
+      <c r="AC136">
+        <v>8028</v>
+      </c>
+      <c r="AD136">
+        <v>0.0</v>
+      </c>
+      <c r="AE136" s="3"/>
+      <c r="AF136">
+        <v>1</v>
+      </c>
+      <c r="AG136" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH136">
+        <v>2</v>
+      </c>
+      <c r="AI136">
+        <v>3864.0</v>
+      </c>
+      <c r="AJ136" s="3"/>
+    </row>
+    <row r="137" spans="1:38">
+      <c r="A137" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C137" s="5">
+        <v>45866.21369213</v>
+      </c>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J137" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K137" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="L137" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M137" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="N137" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="O137" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="P137" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q137" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="R137" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="S137" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T137" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="U137" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V137" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W137">
+        <v>0</v>
+      </c>
+      <c r="X137">
+        <v>0.0</v>
+      </c>
+      <c r="Y137">
+        <v>2760.0</v>
+      </c>
+      <c r="Z137" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA137">
+        <v>300</v>
+      </c>
+      <c r="AB137">
+        <v>0</v>
+      </c>
+      <c r="AC137">
+        <v>3060</v>
+      </c>
+      <c r="AD137">
+        <v>0.0</v>
+      </c>
+      <c r="AE137" s="3"/>
+      <c r="AF137">
+        <v>1</v>
+      </c>
+      <c r="AG137" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="AH137">
+        <v>1</v>
+      </c>
+      <c r="AI137">
+        <v>2760.0</v>
+      </c>
+      <c r="AJ137" s="3"/>
+    </row>
+    <row r="138" spans="1:38">
+      <c r="A138" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C138" s="5">
+        <v>45866.337534722</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M138" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="N138" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="O138" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P138" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="Q138" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="R138" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="S138" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="T138" s="3"/>
+      <c r="U138" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V138" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W138">
+        <v>0</v>
+      </c>
+      <c r="X138">
+        <v>0.0</v>
+      </c>
+      <c r="Y138">
+        <v>3588.0</v>
+      </c>
+      <c r="Z138" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA138">
+        <v>300</v>
+      </c>
+      <c r="AB138">
+        <v>0</v>
+      </c>
+      <c r="AC138">
+        <v>3888</v>
+      </c>
+      <c r="AD138">
+        <v>0.0</v>
+      </c>
+      <c r="AE138" s="3"/>
+      <c r="AF138">
+        <v>1</v>
+      </c>
+      <c r="AG138" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH138">
+        <v>1</v>
+      </c>
+      <c r="AI138">
+        <v>3588.0</v>
+      </c>
+      <c r="AJ138" s="3"/>
+    </row>
+    <row r="139" spans="1:38">
+      <c r="A139" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139" s="5">
+        <v>45867.484791667</v>
+      </c>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G139" s="3"/>
+      <c r="H139" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="J139" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K139" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="L139" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M139" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="N139" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="O139" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="P139" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q139" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="R139" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="S139" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T139" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="U139" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V139" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W139">
+        <v>0</v>
+      </c>
+      <c r="X139">
+        <v>0.0</v>
+      </c>
+      <c r="Y139">
+        <v>8947.0</v>
+      </c>
+      <c r="Z139" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA139">
+        <v>300</v>
+      </c>
+      <c r="AB139">
+        <v>0</v>
+      </c>
+      <c r="AC139">
+        <v>9247</v>
+      </c>
+      <c r="AD139">
+        <v>0.0</v>
+      </c>
+      <c r="AE139" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="AF139" t="s">
+        <v>587</v>
+      </c>
+      <c r="AG139" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="AH139" t="s">
+        <v>589</v>
+      </c>
+      <c r="AI139" t="s">
+        <v>923</v>
+      </c>
+      <c r="AJ139" s="3"/>
+    </row>
+    <row r="140" spans="1:38">
+      <c r="A140" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C140" s="5">
+        <v>45868.209537037</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="L140" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M140" s="3" t="s">
+        <v>931</v>
+      </c>
+      <c r="N140" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="O140" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="P140" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="Q140" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="R140" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="S140" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="T140" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="U140" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V140" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W140">
+        <v>0</v>
+      </c>
+      <c r="X140">
+        <v>0.0</v>
+      </c>
+      <c r="Y140">
+        <v>3588.0</v>
+      </c>
+      <c r="Z140" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA140">
+        <v>300</v>
+      </c>
+      <c r="AB140">
+        <v>0</v>
+      </c>
+      <c r="AC140">
+        <v>3888</v>
+      </c>
+      <c r="AD140">
+        <v>0.0</v>
+      </c>
+      <c r="AE140" s="3"/>
+      <c r="AF140">
+        <v>1</v>
+      </c>
+      <c r="AG140" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH140">
+        <v>1</v>
+      </c>
+      <c r="AI140">
+        <v>3588.0</v>
+      </c>
+      <c r="AJ140" s="3"/>
+    </row>
+    <row r="141" spans="1:38">
+      <c r="A141" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C141" s="5">
+        <v>45868.297164352</v>
+      </c>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="L141" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M141" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="N141" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="O141" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="P141" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="Q141" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="R141" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="S141" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T141" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="U141" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V141" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W141">
+        <v>0</v>
+      </c>
+      <c r="X141">
+        <v>0.0</v>
+      </c>
+      <c r="Y141">
+        <v>65000.0</v>
+      </c>
+      <c r="Z141" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA141">
+        <v>300</v>
+      </c>
+      <c r="AB141">
+        <v>0</v>
+      </c>
+      <c r="AC141">
+        <v>65300</v>
+      </c>
+      <c r="AD141">
+        <v>0.0</v>
+      </c>
+      <c r="AE141" s="3"/>
+      <c r="AF141">
+        <v>1</v>
+      </c>
+      <c r="AG141" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH141">
+        <v>50</v>
+      </c>
+      <c r="AI141">
+        <v>1300.0</v>
+      </c>
+      <c r="AJ141" s="3"/>
+    </row>
+    <row r="142" spans="1:38">
+      <c r="A142" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C142" s="5">
+        <v>45868.705729167</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M142" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="N142" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="O142" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P142" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="Q142" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="R142" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="S142" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T142" s="3"/>
+      <c r="U142" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V142" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W142">
+        <v>0</v>
+      </c>
+      <c r="X142">
+        <v>0.0</v>
+      </c>
+      <c r="Y142">
+        <v>575.0</v>
+      </c>
+      <c r="Z142" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA142">
+        <v>300</v>
+      </c>
+      <c r="AB142">
+        <v>0</v>
+      </c>
+      <c r="AC142">
+        <v>875</v>
+      </c>
+      <c r="AD142">
+        <v>0.0</v>
+      </c>
+      <c r="AE142" s="3"/>
+      <c r="AF142">
+        <v>1</v>
+      </c>
+      <c r="AG142" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH142">
+        <v>1</v>
+      </c>
+      <c r="AI142">
+        <v>575.0</v>
+      </c>
+      <c r="AJ142" s="3"/>
+    </row>
+    <row r="143" spans="1:38">
+      <c r="A143" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C143" s="5">
+        <v>45872.413888889</v>
+      </c>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="J143" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K143" s="3"/>
+      <c r="L143" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M143" s="3"/>
+      <c r="N143" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="O143" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="P143" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="Q143" s="3" t="s">
+        <v>944</v>
+      </c>
+      <c r="R143" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="S143" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T143" s="3"/>
+      <c r="U143" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V143" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W143">
+        <v>0</v>
+      </c>
+      <c r="X143">
+        <v>0.0</v>
+      </c>
+      <c r="Y143">
+        <v>5000.0</v>
+      </c>
+      <c r="Z143" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA143">
+        <v>300</v>
+      </c>
+      <c r="AB143">
+        <v>0</v>
+      </c>
+      <c r="AC143">
+        <v>5300</v>
+      </c>
+      <c r="AD143">
+        <v>0.0</v>
+      </c>
+      <c r="AE143" s="3"/>
+      <c r="AF143">
+        <v>1</v>
+      </c>
+      <c r="AG143" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH143">
+        <v>1</v>
+      </c>
+      <c r="AI143">
+        <v>5000.0</v>
+      </c>
+      <c r="AJ143" s="3"/>
+    </row>
+    <row r="144" spans="1:38">
+      <c r="A144" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C144" s="5">
+        <v>45872.571423611</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="G144" s="3"/>
+      <c r="H144" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M144" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="N144" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="O144" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="P144" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q144" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="R144" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T144" s="3"/>
+      <c r="U144" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W144">
+        <v>0</v>
+      </c>
+      <c r="X144">
+        <v>0.0</v>
+      </c>
+      <c r="Y144">
+        <v>5939.0</v>
+      </c>
+      <c r="Z144" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA144">
+        <v>300</v>
+      </c>
+      <c r="AB144">
+        <v>0</v>
+      </c>
+      <c r="AC144">
+        <v>6239</v>
+      </c>
+      <c r="AD144">
+        <v>0.0</v>
+      </c>
+      <c r="AE144" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="AF144" t="s">
+        <v>587</v>
+      </c>
+      <c r="AG144" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="AH144" t="s">
+        <v>589</v>
+      </c>
+      <c r="AI144" t="s">
+        <v>952</v>
+      </c>
+      <c r="AJ144" s="3"/>
+    </row>
+    <row r="145" spans="1:38">
+      <c r="A145" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C145" s="5">
+        <v>45872.812627315</v>
+      </c>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="G145" s="3"/>
+      <c r="H145" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J145" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="L145" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M145" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="N145" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="O145" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="P145" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q145" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="R145" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="S145" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T145" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="U145" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V145" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W145">
+        <v>0</v>
+      </c>
+      <c r="X145">
+        <v>0.0</v>
+      </c>
+      <c r="Y145">
+        <v>1700.0</v>
+      </c>
+      <c r="Z145" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA145">
+        <v>300</v>
+      </c>
+      <c r="AB145">
+        <v>0</v>
+      </c>
+      <c r="AC145">
+        <v>2000</v>
+      </c>
+      <c r="AD145">
+        <v>0.0</v>
+      </c>
+      <c r="AE145" s="3"/>
+      <c r="AF145">
+        <v>1</v>
+      </c>
+      <c r="AG145" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="AH145">
+        <v>1</v>
+      </c>
+      <c r="AI145">
+        <v>1700.0</v>
+      </c>
+      <c r="AJ145" s="3"/>
+    </row>
+    <row r="146" spans="1:38">
+      <c r="A146" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C146" s="5">
+        <v>45875.238877315</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="F146" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="G146" s="3"/>
+      <c r="H146" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K146" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="L146" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="O146" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="P146" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q146" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="R146" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="S146" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T146" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="U146" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V146" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W146">
+        <v>0</v>
+      </c>
+      <c r="X146">
+        <v>0.0</v>
+      </c>
+      <c r="Y146">
+        <v>8740.0</v>
+      </c>
+      <c r="Z146" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA146">
+        <v>300</v>
+      </c>
+      <c r="AB146">
+        <v>0</v>
+      </c>
+      <c r="AC146">
+        <v>9040</v>
+      </c>
+      <c r="AD146">
+        <v>0.0</v>
+      </c>
+      <c r="AE146" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF146" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG146" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="AH146" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI146" t="s">
+        <v>965</v>
+      </c>
+      <c r="AJ146" s="3"/>
+    </row>
+    <row r="147" spans="1:38">
+      <c r="A147" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C147" s="5">
+        <v>45876.222962963</v>
+      </c>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M147" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="N147" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="O147" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="P147" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q147" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="R147" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="S147" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T147" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="U147" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V147" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W147">
+        <v>0</v>
+      </c>
+      <c r="X147">
+        <v>0.0</v>
+      </c>
+      <c r="Y147">
+        <v>2600.0</v>
+      </c>
+      <c r="Z147" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA147">
+        <v>300</v>
+      </c>
+      <c r="AB147">
+        <v>0</v>
+      </c>
+      <c r="AC147">
+        <v>2900</v>
+      </c>
+      <c r="AD147">
+        <v>0.0</v>
+      </c>
+      <c r="AE147" s="3"/>
+      <c r="AF147">
+        <v>1</v>
+      </c>
+      <c r="AG147" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH147">
+        <v>2</v>
+      </c>
+      <c r="AI147">
+        <v>1300.0</v>
+      </c>
+      <c r="AJ147" s="3"/>
+    </row>
+    <row r="148" spans="1:38">
+      <c r="A148" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C148" s="5">
+        <v>45876.629074074</v>
+      </c>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M148" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="N148" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="O148" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="P148" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q148" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="R148" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="S148" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T148" s="3"/>
+      <c r="U148" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V148" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W148">
+        <v>0</v>
+      </c>
+      <c r="X148">
+        <v>0.0</v>
+      </c>
+      <c r="Y148">
+        <v>5364.0</v>
+      </c>
+      <c r="Z148" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA148">
+        <v>300</v>
+      </c>
+      <c r="AB148">
+        <v>0</v>
+      </c>
+      <c r="AC148">
+        <v>5664</v>
+      </c>
+      <c r="AD148">
+        <v>0.0</v>
+      </c>
+      <c r="AE148" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF148" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG148" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH148" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI148" t="s">
+        <v>277</v>
+      </c>
+      <c r="AJ148" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>